<commit_message>
auto column width, extract live value
</commit_message>
<xml_diff>
--- a/Sigma Stock/bogdan.popa.g25@gmail.com.xlsx
+++ b/Sigma Stock/bogdan.popa.g25@gmail.com.xlsx
@@ -1,16 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <x:workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Z\UiPath Studio\Sigma Stock Bot\Sigma Stock\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0178219F-CA9C-4039-89D3-2C5104208333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView firstSheet="0" activeTab="0"/>
+    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="META" sheetId="2" r:id="rId2"/>
-    <x:sheet name="MCHVF" sheetId="5" r:id="rId5"/>
+    <x:sheet name="META" sheetId="2" r:id="rId1"/>
+    <x:sheet name="MCHVF" sheetId="5" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="125725"/>
+  <x:calcPr calcId="0"/>
 </x:workbook>
 </file>
 
@@ -32,13 +39,13 @@
     <x:t>Bid</x:t>
   </x:si>
   <x:si>
-    <x:t>120.65 x 800</x:t>
+    <x:t>120.15 x 800</x:t>
   </x:si>
   <x:si>
     <x:t>Ask</x:t>
   </x:si>
   <x:si>
-    <x:t>120.84 x 1000</x:t>
+    <x:t>120.42 x 1000</x:t>
   </x:si>
   <x:si>
     <x:t>Day's Range</x:t>
@@ -89,13 +96,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1">
+  <x:fonts count="1" x14ac:knownFonts="1">
     <x:font>
-      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -111,38 +117,32 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
     </x:border>
   </x:borders>
   <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </x:cellStyleXfs>
   <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </x:ext>
+  </x:extLst>
 </x:styleSheet>
 </file>
 
@@ -430,17 +430,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
   <x:dimension ref="A1:B8"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
+    <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <x:sheetData>
-    <x:row r="1" spans="1:2">
+    <x:row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -448,7 +448,7 @@
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:2">
+    <x:row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
@@ -456,7 +456,7 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:2">
+    <x:row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A3" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -464,7 +464,7 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:2">
+    <x:row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A4" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -472,7 +472,7 @@
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:2">
+    <x:row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A5" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
@@ -480,7 +480,7 @@
         <x:v>9</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:2">
+    <x:row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A6" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -488,7 +488,7 @@
         <x:v>11</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:2">
+    <x:row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A7" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -496,7 +496,7 @@
         <x:v>13</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:2">
+    <x:row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A8" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -514,7 +514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0100-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -522,9 +522,9 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <x:sheetData>
-    <x:row r="1" spans="1:2">
+    <x:row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -532,7 +532,7 @@
         <x:v>16</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:2">
+    <x:row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
@@ -540,7 +540,7 @@
         <x:v>17</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:2">
+    <x:row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A3" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -548,7 +548,7 @@
         <x:v>18</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:2">
+    <x:row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A4" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -556,7 +556,7 @@
         <x:v>18</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:2">
+    <x:row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A5" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
@@ -564,7 +564,7 @@
         <x:v>19</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:2">
+    <x:row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A6" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -572,7 +572,7 @@
         <x:v>20</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:2">
+    <x:row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A7" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -580,7 +580,7 @@
         <x:v>21</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:2">
+    <x:row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A8" s="0" t="s">
         <x:v>14</x:v>
       </x:c>

</xml_diff>